<commit_message>
fix login complete index
</commit_message>
<xml_diff>
--- a/doing.xlsx
+++ b/doing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Tài </t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Login bằng Token key</t>
+  </si>
+  <si>
+    <t>Xong giao diện</t>
+  </si>
+  <si>
+    <t>Fix lỗi login Token, http headers</t>
   </si>
 </sst>
 </file>
@@ -80,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -94,6 +100,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D6"/>
+  <dimension ref="A5:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -439,7 +448,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>43531</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>